<commit_message>
Added Position class and some changes.
</commit_message>
<xml_diff>
--- a/TelerikProject.xlsx
+++ b/TelerikProject.xlsx
@@ -2,10 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GIT\Source\Repos\Telerik-Academy\Module 1 - OOP - Teamwork\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_telerik\OOP_Teamwork\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Q-s" sheetId="3" r:id="rId3"/>
     <sheet name="PartCategory" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="92">
   <si>
     <t>Employee</t>
   </si>
@@ -84,9 +84,6 @@
     <t>PaymentType</t>
   </si>
   <si>
-    <t>PaySalary</t>
-  </si>
-  <si>
     <t>Pay &lt;= static?</t>
   </si>
   <si>
@@ -102,9 +99,6 @@
     <t>Properties</t>
   </si>
   <si>
-    <t>AddPosition</t>
-  </si>
-  <si>
     <t>Interface</t>
   </si>
   <si>
@@ -132,12 +126,6 @@
     <t>SetLocation</t>
   </si>
   <si>
-    <t>CreditLimit</t>
-  </si>
-  <si>
-    <t>OutstandingLimit</t>
-  </si>
-  <si>
     <t>Angel</t>
   </si>
   <si>
@@ -145,11 +133,6 @@
   </si>
   <si>
     <t>Part</t>
-  </si>
-  <si>
-    <t>Name, 
-Address, 
-TaxNumber</t>
   </si>
   <si>
     <t>specific service info - address, 
@@ -159,14 +142,6 @@
 List of Employees</t>
   </si>
   <si>
-    <t>SendReminderForOutstandingInvoices, 
-SetCreditLimit</t>
-  </si>
-  <si>
-    <t>PayInvoices, 
-AddVendor</t>
-  </si>
-  <si>
     <t>Pay.Salary, 
 Pay.Invoices</t>
   </si>
@@ -196,40 +171,6 @@
   </si>
   <si>
     <t>Answer</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Name,
-Age,
-ServiceStore, 
-Salary, 
-Position, 
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>WorkingType</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>, 
-PersonalPhone</t>
-    </r>
   </si>
   <si>
     <t>Interior</t>
@@ -416,11 +357,73 @@
       <t>PartMountTime - employee confirms what is the time required to mount the part on this specific car model</t>
     </r>
   </si>
+  <si>
+    <t>Alex</t>
+  </si>
+  <si>
+    <t>Iemployee</t>
+  </si>
+  <si>
+    <t>ChangeSalary, ChangePosition, FireEmployee</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">FirstName, LastName,
+ServiceStore, 
+Salary, 
+Position, 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>WorkingType</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, IsStillHired</t>
+    </r>
+  </si>
+  <si>
+    <t>Name, 
+Address, 
+TaxNumber, uniqueNumber, creditLimit, Invoices</t>
+  </si>
+  <si>
+    <t>dueDaysAllowed</t>
+  </si>
+  <si>
+    <t>SendReminderForOutstandingInvoices, 
+UpdateCreditLimit</t>
+  </si>
+  <si>
+    <t>UpdateCreditLimit, ChangeAddress, ChangeTaxNumber</t>
+  </si>
+  <si>
+    <t>IVendor</t>
+  </si>
+  <si>
+    <t>IClient</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -543,7 +546,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -572,6 +575,20 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -898,50 +915,51 @@
   <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="7.140625" style="6" customWidth="1"/>
     <col min="3" max="3" width="31.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="73.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="70.42578125" style="4" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="31.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="69.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="36.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5703125" style="4" bestFit="1" customWidth="1"/>
     <col min="8" max="10" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C1" s="7" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="D1"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C2" s="3" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="D2"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C3" s="8" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="D3"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>4</v>
@@ -950,128 +968,176 @@
         <v>3</v>
       </c>
       <c r="G5" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" s="14" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A6" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="B6" s="12"/>
+      <c r="C6" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" ht="105" x14ac:dyDescent="0.25">
-      <c r="C6" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="E6" s="4" t="s">
+      <c r="F6" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="H6" s="13"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="13"/>
+    </row>
+    <row r="7" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="B7" s="15"/>
+      <c r="C7" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="16"/>
+      <c r="I7" s="16"/>
+      <c r="J7" s="16"/>
+    </row>
+    <row r="8" spans="1:10" s="14" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="B8" s="12"/>
+      <c r="C8" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H8" s="13"/>
+      <c r="I8" s="13"/>
+      <c r="J8" s="13"/>
+    </row>
+    <row r="9" spans="1:10" s="14" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="B9" s="12"/>
+      <c r="C9" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="H9" s="13"/>
+      <c r="I9" s="13"/>
+      <c r="J9" s="13"/>
+    </row>
+    <row r="10" spans="1:10" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="B10" s="12"/>
+      <c r="C10" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="D10" s="3"/>
+      <c r="E10" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="H10" s="13"/>
+      <c r="I10" s="13"/>
+      <c r="J10" s="13"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C12" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+      <c r="C13" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="C14" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C7" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="C8" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="C9" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D9" s="4" t="s">
+      <c r="F14" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="150" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="F9" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="C10" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C11" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="C12" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="C13" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C14" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="150" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>26</v>
-      </c>
       <c r="D15" s="3" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="C16" s="4" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -1098,51 +1164,51 @@
   <sheetData>
     <row r="1" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B1" s="11" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -1165,10 +1231,10 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -1177,10 +1243,10 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -1188,13 +1254,13 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="C4" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="H4" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="I4" t="str">
         <f>H4&amp;","</f>
@@ -1203,10 +1269,10 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="H5" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="I5" t="str">
         <f>H5&amp;","</f>
@@ -1218,13 +1284,13 @@
         <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="C7" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="H7" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="I7" t="str">
         <f t="shared" ref="I7:I17" si="0">H7&amp;","</f>
@@ -1233,10 +1299,10 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="H8" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="I8" t="str">
         <f t="shared" si="0"/>
@@ -1245,10 +1311,10 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="H9" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="I9" t="str">
         <f t="shared" si="0"/>
@@ -1257,10 +1323,10 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="H10" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="I10" t="str">
         <f t="shared" si="0"/>
@@ -1269,10 +1335,10 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="H11" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="I11" t="str">
         <f t="shared" si="0"/>
@@ -1281,10 +1347,10 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="H12" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="I12" t="str">
         <f t="shared" si="0"/>
@@ -1293,10 +1359,10 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="H13" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="I13" t="str">
         <f t="shared" si="0"/>
@@ -1305,10 +1371,10 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="H14" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="I14" t="str">
         <f t="shared" si="0"/>
@@ -1317,10 +1383,10 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="H15" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="I15" t="str">
         <f t="shared" si="0"/>
@@ -1329,10 +1395,10 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="H16" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="I16" t="str">
         <f t="shared" si="0"/>
@@ -1341,10 +1407,10 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="H17" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="I17" t="str">
         <f t="shared" si="0"/>
@@ -1356,13 +1422,13 @@
         <v>3</v>
       </c>
       <c r="B19" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="C19" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="H19" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="I19" t="str">
         <f t="shared" ref="I19:I21" si="1">H19&amp;","</f>
@@ -1371,10 +1437,10 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="H20" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="I20" t="str">
         <f t="shared" si="1"/>
@@ -1383,10 +1449,10 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="H21" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="I21" t="str">
         <f t="shared" si="1"/>
@@ -1398,13 +1464,13 @@
         <v>4</v>
       </c>
       <c r="B23" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="C23" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="H23" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="I23" t="str">
         <f t="shared" ref="I23:I30" si="2">H23&amp;","</f>
@@ -1413,10 +1479,10 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C24" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="H24" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="I24" t="str">
         <f t="shared" si="2"/>
@@ -1425,10 +1491,10 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="H25" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="I25" t="str">
         <f t="shared" si="2"/>
@@ -1437,10 +1503,10 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C26" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="H26" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="I26" t="str">
         <f t="shared" si="2"/>
@@ -1449,10 +1515,10 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="H27" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="I27" t="str">
         <f t="shared" si="2"/>
@@ -1461,10 +1527,10 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C28" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="H28" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="I28" t="str">
         <f t="shared" si="2"/>
@@ -1473,10 +1539,10 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C29" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="H29" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="I29" t="str">
         <f t="shared" si="2"/>
@@ -1485,10 +1551,10 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C30" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="H30" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="I30" t="str">
         <f t="shared" si="2"/>
@@ -1500,13 +1566,13 @@
         <v>5</v>
       </c>
       <c r="B32" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="C32" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="H32" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="I32" t="str">
         <f t="shared" ref="I32:I35" si="3">H32&amp;","</f>
@@ -1515,10 +1581,10 @@
     </row>
     <row r="33" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C33" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="H33" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="I33" t="str">
         <f t="shared" si="3"/>
@@ -1527,10 +1593,10 @@
     </row>
     <row r="34" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C34" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="H34" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="I34" t="str">
         <f t="shared" si="3"/>
@@ -1539,10 +1605,10 @@
     </row>
     <row r="35" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C35" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="H35" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="I35" t="str">
         <f t="shared" si="3"/>

</xml_diff>